<commit_message>
Changes done for image upload
</commit_message>
<xml_diff>
--- a/src/test/resources/GorestUserData.xlsx
+++ b/src/test/resources/GorestUserData.xlsx
@@ -102,16 +102,16 @@
     <t>19-09-1987</t>
   </si>
   <si>
-    <t>abc1@gmail.com</t>
-  </si>
-  <si>
-    <t>abc2@gmail.com</t>
-  </si>
-  <si>
-    <t>abc3@gmail.com</t>
-  </si>
-  <si>
-    <t>abc4@gmail.com</t>
+    <t>abc5@gmail.com</t>
+  </si>
+  <si>
+    <t>abc6@gmail.com</t>
+  </si>
+  <si>
+    <t>abc7@gmail.com</t>
+  </si>
+  <si>
+    <t>abc8@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>